<commit_message>
update graphs and tables
</commit_message>
<xml_diff>
--- a/supplementary_data/area_pop_sums.xlsx
+++ b/supplementary_data/area_pop_sums.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="162">
   <si>
     <t>Coastal and marine Ecosystems</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Terrestrial ecosystems</t>
   </si>
   <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>area</t>
   </si>
   <si>
@@ -55,46 +58,55 @@
     <t>Oceania</t>
   </si>
   <si>
+    <t>Global</t>
+  </si>
+  <si>
     <t>D&amp;A</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
-    <t>8% (5%-30%)</t>
-  </si>
-  <si>
-    <t>4% (2%-27%)</t>
-  </si>
-  <si>
-    <t>34% (22%-49%)</t>
-  </si>
-  <si>
-    <t>11% (5%-11%)</t>
-  </si>
-  <si>
-    <t>13% (5%-25%)</t>
+    <t>8% (5%-31%)</t>
+  </si>
+  <si>
+    <t>3% (1%-27%)</t>
+  </si>
+  <si>
+    <t>33% (19%-50%)</t>
+  </si>
+  <si>
+    <t>11% (5%-12%)</t>
+  </si>
+  <si>
+    <t>12% (4%-23%)</t>
   </si>
   <si>
     <t>2% (0%-4%)</t>
   </si>
   <si>
-    <t>18% (13%-24%)</t>
+    <t>16% (11%-21%)</t>
   </si>
   <si>
     <t>0% (0%-0%)</t>
   </si>
   <si>
-    <t>23% (9%-32%)</t>
-  </si>
-  <si>
-    <t>4% (1%-5%)</t>
-  </si>
-  <si>
-    <t>71% (63%-72%)</t>
-  </si>
-  <si>
-    <t>14% (13%-14%)</t>
+    <t>19% (6%-29%)</t>
+  </si>
+  <si>
+    <t>3% (1%-4%)</t>
+  </si>
+  <si>
+    <t>76% (72%-76%)</t>
+  </si>
+  <si>
+    <t>14% (14%-14%)</t>
+  </si>
+  <si>
+    <t>22% (13%-33%)</t>
+  </si>
+  <si>
+    <t>5% (2%-8%)</t>
   </si>
   <si>
     <t>26% (18%-51%)</t>
@@ -130,40 +142,49 @@
     <t>5% (5%-5%)</t>
   </si>
   <si>
-    <t>27% (13%-61%)</t>
-  </si>
-  <si>
-    <t>24% (6%-34%)</t>
-  </si>
-  <si>
-    <t>37% (23%-56%)</t>
-  </si>
-  <si>
-    <t>8% (7%-15%)</t>
-  </si>
-  <si>
-    <t>32% (25%-47%)</t>
-  </si>
-  <si>
-    <t>7% (3%-13%)</t>
-  </si>
-  <si>
-    <t>26% (22%-34%)</t>
+    <t>44% (23%-57%)</t>
+  </si>
+  <si>
+    <t>8% (3%-11%)</t>
+  </si>
+  <si>
+    <t>26% (13%-62%)</t>
+  </si>
+  <si>
+    <t>24% (5%-34%)</t>
+  </si>
+  <si>
+    <t>40% (25%-57%)</t>
+  </si>
+  <si>
+    <t>9% (7%-15%)</t>
+  </si>
+  <si>
+    <t>32% (25%-46%)</t>
+  </si>
+  <si>
+    <t>7% (3%-14%)</t>
+  </si>
+  <si>
+    <t>25% (20%-33%)</t>
   </si>
   <si>
     <t>1% (0%-1%)</t>
   </si>
   <si>
-    <t>62% (46%-77%)</t>
-  </si>
-  <si>
-    <t>6% (6%-9%)</t>
-  </si>
-  <si>
-    <t>66% (47%-77%)</t>
-  </si>
-  <si>
-    <t>13% (13%-13%)</t>
+    <t>61% (44%-78%)</t>
+  </si>
+  <si>
+    <t>5% (5%-7%)</t>
+  </si>
+  <si>
+    <t>74% (53%-84%)</t>
+  </si>
+  <si>
+    <t>38% (27%-53%)</t>
+  </si>
+  <si>
+    <t>8% (4%-12%)</t>
   </si>
   <si>
     <t>55% (38%-79%)</t>
@@ -196,16 +217,22 @@
     <t>70% (54%-86%)</t>
   </si>
   <si>
-    <t>11% (9%-16%)</t>
-  </si>
-  <si>
-    <t>13% (5%-14%)</t>
-  </si>
-  <si>
-    <t>31% (17%-51%)</t>
-  </si>
-  <si>
-    <t>7% (4%-19%)</t>
+    <t>73% (64%-79%)</t>
+  </si>
+  <si>
+    <t>11% (11%-12%)</t>
+  </si>
+  <si>
+    <t>11% (8%-15%)</t>
+  </si>
+  <si>
+    <t>13% (6%-14%)</t>
+  </si>
+  <si>
+    <t>34% (18%-54%)</t>
+  </si>
+  <si>
+    <t>8% (5%-19%)</t>
   </si>
   <si>
     <t>3% (1%-9%)</t>
@@ -214,19 +241,25 @@
     <t>0% (0%-1%)</t>
   </si>
   <si>
-    <t>22% (9%-31%)</t>
-  </si>
-  <si>
-    <t>26% (14%-41%)</t>
-  </si>
-  <si>
-    <t>4% (2%-5%)</t>
-  </si>
-  <si>
-    <t>5% (2%-9%)</t>
-  </si>
-  <si>
-    <t>3% (3%-4%)</t>
+    <t>21% (8%-30%)</t>
+  </si>
+  <si>
+    <t>27% (14%-43%)</t>
+  </si>
+  <si>
+    <t>4% (2%-4%)</t>
+  </si>
+  <si>
+    <t>3% (2%-8%)</t>
+  </si>
+  <si>
+    <t>1% (1%-3%)</t>
+  </si>
+  <si>
+    <t>17% (9%-27%)</t>
+  </si>
+  <si>
+    <t>4% (2%-7%)</t>
   </si>
   <si>
     <t>19% (14%-32%)</t>
@@ -259,40 +292,46 @@
     <t>4% (4%-4%)</t>
   </si>
   <si>
-    <t>17% (7%-44%)</t>
-  </si>
-  <si>
-    <t>18% (3%-33%)</t>
-  </si>
-  <si>
-    <t>47% (22%-61%)</t>
-  </si>
-  <si>
-    <t>14% (8%-17%)</t>
-  </si>
-  <si>
-    <t>18% (5%-36%)</t>
+    <t>32% (13%-46%)</t>
+  </si>
+  <si>
+    <t>9% (4%-10%)</t>
+  </si>
+  <si>
+    <t>16% (6%-45%)</t>
+  </si>
+  <si>
+    <t>19% (3%-34%)</t>
+  </si>
+  <si>
+    <t>52% (24%-64%)</t>
+  </si>
+  <si>
+    <t>15% (9%-18%)</t>
+  </si>
+  <si>
+    <t>17% (5%-35%)</t>
   </si>
   <si>
     <t>9% (1%-13%)</t>
   </si>
   <si>
-    <t>26% (19%-33%)</t>
-  </si>
-  <si>
-    <t>1% (1%-1%)</t>
-  </si>
-  <si>
-    <t>59% (32%-71%)</t>
-  </si>
-  <si>
-    <t>6% (5%-7%)</t>
-  </si>
-  <si>
-    <t>18% (4%-71%)</t>
-  </si>
-  <si>
-    <t>13% (3%-13%)</t>
+    <t>24% (18%-31%)</t>
+  </si>
+  <si>
+    <t>61% (34%-72%)</t>
+  </si>
+  <si>
+    <t>19% (4%-83%)</t>
+  </si>
+  <si>
+    <t>14% (1%-14%)</t>
+  </si>
+  <si>
+    <t>32% (16%-49%)</t>
+  </si>
+  <si>
+    <t>9% (3%-12%)</t>
   </si>
   <si>
     <t>33% (14%-68%)</t>
@@ -310,9 +349,6 @@
     <t>44% (18%-68%)</t>
   </si>
   <si>
-    <t>4% (2%-7%)</t>
-  </si>
-  <si>
     <t>77% (64%-86%)</t>
   </si>
   <si>
@@ -325,37 +361,46 @@
     <t>5% (4%-5%)</t>
   </si>
   <si>
-    <t>64% (38%-64%)</t>
-  </si>
-  <si>
-    <t>35% (29%-35%)</t>
-  </si>
-  <si>
-    <t>69% (59%-70%)</t>
+    <t>62% (40%-75%)</t>
+  </si>
+  <si>
+    <t>11% (10%-12%)</t>
+  </si>
+  <si>
+    <t>63% (38%-64%)</t>
+  </si>
+  <si>
+    <t>36% (29%-36%)</t>
+  </si>
+  <si>
+    <t>70% (61%-70%)</t>
   </si>
   <si>
     <t>21% (16%-21%)</t>
   </si>
   <si>
-    <t>42% (23%-52%)</t>
-  </si>
-  <si>
-    <t>7% (2%-19%)</t>
-  </si>
-  <si>
-    <t>36% (30%-57%)</t>
-  </si>
-  <si>
-    <t>1% (0%-3%)</t>
-  </si>
-  <si>
-    <t>70% (58%-80%)</t>
-  </si>
-  <si>
-    <t>7% (5%-9%)</t>
-  </si>
-  <si>
-    <t>73% (65%-78%)</t>
+    <t>40% (22%-51%)</t>
+  </si>
+  <si>
+    <t>7% (3%-20%)</t>
+  </si>
+  <si>
+    <t>35% (28%-56%)</t>
+  </si>
+  <si>
+    <t>71% (60%-81%)</t>
+  </si>
+  <si>
+    <t>6% (4%-7%)</t>
+  </si>
+  <si>
+    <t>84% (79%-86%)</t>
+  </si>
+  <si>
+    <t>53% (41%-62%)</t>
+  </si>
+  <si>
+    <t>12% (9%-15%)</t>
   </si>
   <si>
     <t>77% (67%-81%)</t>
@@ -383,6 +428,78 @@
   </si>
   <si>
     <t>77% (74%-92%)</t>
+  </si>
+  <si>
+    <t>75% (63%-81%)</t>
+  </si>
+  <si>
+    <t>12% (11%-13%)</t>
+  </si>
+  <si>
+    <t>52% (18%-63%)</t>
+  </si>
+  <si>
+    <t>33% (12%-36%)</t>
+  </si>
+  <si>
+    <t>62% (55%-70%)</t>
+  </si>
+  <si>
+    <t>17% (16%-21%)</t>
+  </si>
+  <si>
+    <t>32% (24%-41%)</t>
+  </si>
+  <si>
+    <t>6% (2%-12%)</t>
+  </si>
+  <si>
+    <t>28% (25%-34%)</t>
+  </si>
+  <si>
+    <t>70% (60%-76%)</t>
+  </si>
+  <si>
+    <t>5% (5%-6%)</t>
+  </si>
+  <si>
+    <t>84% (74%-86%)</t>
+  </si>
+  <si>
+    <t>48% (37%-56%)</t>
+  </si>
+  <si>
+    <t>10% (6%-13%)</t>
+  </si>
+  <si>
+    <t>75% (46%-81%)</t>
+  </si>
+  <si>
+    <t>19% (13%-19%)</t>
+  </si>
+  <si>
+    <t>70% (69%-72%)</t>
+  </si>
+  <si>
+    <t>66% (51%-75%)</t>
+  </si>
+  <si>
+    <t>4% (2%-6%)</t>
+  </si>
+  <si>
+    <t>83% (78%-90%)</t>
+  </si>
+  <si>
+    <t>80% (78%-82%)</t>
+  </si>
+  <si>
+    <t>84% (75%-92%)</t>
+  </si>
+  <si>
+    <t>74% (67%-80%)</t>
+  </si>
+  <si>
+    <t>12% (11%-12%)</t>
   </si>
 </sst>
 </file>
@@ -740,13 +857,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -768,497 +885,667 @@
         <v>4</v>
       </c>
       <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="L4" t="s">
-        <v>114</v>
+        <v>129</v>
+      </c>
+      <c r="M4" t="s">
+        <v>140</v>
+      </c>
+      <c r="N4" t="s">
+        <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="J5" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="K5" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="L5" t="s">
-        <v>115</v>
+        <v>130</v>
+      </c>
+      <c r="M5" t="s">
+        <v>141</v>
+      </c>
+      <c r="N5" t="s">
+        <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="L6" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="M6" t="s">
+        <v>142</v>
+      </c>
+      <c r="N6" t="s">
+        <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:14">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="J7" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="K7" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="L7" t="s">
-        <v>96</v>
+        <v>109</v>
+      </c>
+      <c r="M7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N7" t="s">
+        <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I8" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="J8" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="K8" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="L8" t="s">
-        <v>117</v>
+        <v>132</v>
+      </c>
+      <c r="M8" t="s">
+        <v>144</v>
+      </c>
+      <c r="N8" t="s">
+        <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:14">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="J9" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="K9" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="L9" t="s">
-        <v>118</v>
+        <v>133</v>
+      </c>
+      <c r="M9" t="s">
+        <v>145</v>
+      </c>
+      <c r="N9" t="s">
+        <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="I10" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="J10" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="K10" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="L10" t="s">
-        <v>119</v>
+        <v>134</v>
+      </c>
+      <c r="M10" t="s">
+        <v>146</v>
+      </c>
+      <c r="N10" t="s">
+        <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:14">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" t="s">
         <v>88</v>
       </c>
-      <c r="J11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" t="s">
-        <v>110</v>
-      </c>
-      <c r="L11" t="s">
-        <v>22</v>
+      <c r="I12" t="s">
+        <v>101</v>
+      </c>
+      <c r="J12" t="s">
+        <v>112</v>
+      </c>
+      <c r="K12" t="s">
+        <v>124</v>
+      </c>
+      <c r="L12" t="s">
+        <v>135</v>
+      </c>
+      <c r="M12" t="s">
+        <v>147</v>
+      </c>
+      <c r="N12" t="s">
+        <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" t="s">
-        <v>89</v>
-      </c>
-      <c r="J12" t="s">
-        <v>100</v>
-      </c>
-      <c r="K12" t="s">
-        <v>111</v>
-      </c>
-      <c r="L12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:14">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="H13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" t="s">
+        <v>125</v>
+      </c>
+      <c r="L13" t="s">
+        <v>136</v>
+      </c>
+      <c r="M13" t="s">
+        <v>148</v>
+      </c>
+      <c r="N13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" t="s">
         <v>78</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H14" t="s">
         <v>90</v>
       </c>
-      <c r="J13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13" t="s">
-        <v>112</v>
-      </c>
-      <c r="L13" t="s">
-        <v>121</v>
+      <c r="I14" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" t="s">
+        <v>113</v>
+      </c>
+      <c r="K14" t="s">
+        <v>126</v>
+      </c>
+      <c r="L14" t="s">
+        <v>137</v>
+      </c>
+      <c r="M14" t="s">
+        <v>149</v>
+      </c>
+      <c r="N14" t="s">
+        <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" t="s">
-        <v>91</v>
-      </c>
-      <c r="J14" t="s">
-        <v>101</v>
-      </c>
-      <c r="K14" t="s">
-        <v>113</v>
-      </c>
-      <c r="L14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:14">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" t="s">
+        <v>41</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" t="s">
         <v>80</v>
       </c>
-      <c r="I15" t="s">
+      <c r="H16" t="s">
         <v>92</v>
       </c>
-      <c r="J15" t="s">
-        <v>102</v>
-      </c>
-      <c r="K15" t="s">
-        <v>49</v>
-      </c>
-      <c r="L15" t="s">
-        <v>37</v>
+      <c r="I16" t="s">
+        <v>104</v>
+      </c>
+      <c r="J16" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" t="s">
+        <v>127</v>
+      </c>
+      <c r="L16" t="s">
+        <v>138</v>
+      </c>
+      <c r="M16" t="s">
+        <v>150</v>
+      </c>
+      <c r="N16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
+        <v>105</v>
+      </c>
+      <c r="J17" t="s">
+        <v>116</v>
+      </c>
+      <c r="K17" t="s">
+        <v>128</v>
+      </c>
+      <c r="L17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M17" t="s">
+        <v>151</v>
+      </c>
+      <c r="N17" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>